<commit_message>
test QA, report generation
</commit_message>
<xml_diff>
--- a/documents/testerror.xlsx
+++ b/documents/testerror.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn_000\Documents\GitHub\data_portal\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1326437E-A0BB-4E36-8816-C83CF6EE0FF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="147">
   <si>
     <t>sheet</t>
   </si>
@@ -468,15 +469,9 @@
     </r>
   </si>
   <si>
-    <t>Miguelito Lonneman</t>
-  </si>
-  <si>
     <t>testytest@test.edu</t>
   </si>
   <si>
-    <t>Jon Leftneck</t>
-  </si>
-  <si>
     <t>USA-MDA</t>
   </si>
   <si>
@@ -597,13 +592,16 @@
     <t>Spicy plant</t>
   </si>
   <si>
-    <t>CANDY-LAND</t>
+    <t>Jon Lefcheck</t>
+  </si>
+  <si>
+    <t>Michael Lonneman</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -1218,6 +1216,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1253,6 +1268,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1428,14 +1460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="39.950000000000003" customHeight="1"/>
@@ -1462,7 +1494,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1470,7 +1502,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1478,7 +1510,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1494,7 +1526,7 @@
         <v>66</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1554,19 +1586,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="195" yWindow="491" count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of any other person(s) involved" sqref="A7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the protocol" sqref="A2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A10"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A11"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A9" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of any other person(s) involved" sqref="A7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A8" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the protocol" sqref="A2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A10" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A11" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1574,15 +1606,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1634,10 +1666,10 @@
         <v>43656</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16">
         <v>1</v>
@@ -1646,7 +1678,7 @@
         <v>34234523</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1891,21 +1923,21 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="E1 G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="F1 H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="I1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any comments reguarding the sampling location" sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="E1 G1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="F1 H1" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="I1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any comments reguarding the sampling location" sqref="J1" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -1953,10 +1985,10 @@
         <v>43656</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16">
         <v>1</v>
@@ -1965,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1976,10 +2008,10 @@
         <v>43656</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="16">
         <v>1</v>
@@ -1988,7 +2020,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -1999,10 +2031,10 @@
         <v>43656</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="16">
         <v>1</v>
@@ -2011,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -2022,10 +2054,10 @@
         <v>43656</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
@@ -2034,7 +2066,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -2045,10 +2077,10 @@
         <v>43656</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="16">
         <v>1</v>
@@ -2057,7 +2089,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -2068,10 +2100,10 @@
         <v>43656</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="16">
         <v>1</v>
@@ -2080,7 +2112,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -2091,10 +2123,10 @@
         <v>43656</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
@@ -2103,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -2114,10 +2146,10 @@
         <v>43656</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -2126,7 +2158,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2137,10 +2169,10 @@
         <v>43656</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2149,7 +2181,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -2358,20 +2390,20 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover codes are 1, 2, 3, 4, 5 where:_x000d__x000a_1 = 0-5%_x000d__x000a_2 = 5-25%_x000d__x000a_3 = 25-50%_x000d__x000a_4 = 50-75%_x000d__x000a_5 = 75-100%" sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cover codes are 1, 2, 3, 4, 5 where:_x000d__x000a_1 = 0-5%_x000d__x000a_2 = 5-25%_x000d__x000a_3 = 25-50%_x000d__x000a_4 = 50-75%_x000d__x000a_5 = 75-100%" sqref="G1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2428,10 +2460,10 @@
         <v>43656</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16">
         <v>1</v>
@@ -2440,13 +2472,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I2" s="1">
         <v>3245</v>
@@ -2460,10 +2492,10 @@
         <v>43656</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="16">
         <v>1</v>
@@ -2472,13 +2504,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G3" s="1">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -2492,10 +2524,10 @@
         <v>43656</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="16">
         <v>1</v>
@@ -2504,13 +2536,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G4" s="1">
         <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -2524,10 +2556,10 @@
         <v>43656</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
@@ -2536,13 +2568,13 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -2556,10 +2588,10 @@
         <v>43656</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="16">
         <v>1</v>
@@ -2568,19 +2600,19 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2588,10 +2620,10 @@
         <v>43656</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="16">
         <v>1</v>
@@ -2600,13 +2632,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G7" s="1">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I7" s="1">
         <v>4</v>
@@ -2620,10 +2652,10 @@
         <v>43656</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
@@ -2632,19 +2664,19 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8" s="1">
         <v>651</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I8" s="1">
         <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2652,10 +2684,10 @@
         <v>43656</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -2664,13 +2696,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -2684,10 +2716,10 @@
         <v>43656</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2696,13 +2728,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -2914,22 +2946,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1:G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Were there obivious grazing scars present in the quadrat, Y or N?" sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass shoots within the quadrat." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass flowers (if any) present  within the qudrat._x000d__x000a__x000d__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="I1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass fruits (if any) present  within the qudrat._x000a__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1:G1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Were there obivious grazing scars present in the quadrat, Y or N?" sqref="H1" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass shoots within the quadrat." sqref="G1" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass flowers (if any) present  within the qudrat._x000d__x000a__x000d__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="I1" xr:uid="{00000000-0002-0000-0300-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The count of seagrass fruits (if any) present  within the qudrat._x000a__x000a_Remember - Zeros are data! Please enter 0 if no seagrass flowers were present." sqref="J1" xr:uid="{00000000-0002-0000-0300-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0300-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0300-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0300-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0300-000008000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2977,10 +3009,10 @@
         <v>43656</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="16">
         <v>1</v>
@@ -2989,7 +3021,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -3000,10 +3032,10 @@
         <v>43656</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="16">
         <v>1</v>
@@ -3012,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -3023,10 +3055,10 @@
         <v>43656</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="16">
         <v>1</v>
@@ -3035,7 +3067,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -3046,10 +3078,10 @@
         <v>43656</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
@@ -3058,7 +3090,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G5">
         <v>12</v>
@@ -3069,10 +3101,10 @@
         <v>43656</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="16">
         <v>1</v>
@@ -3081,7 +3113,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -3092,10 +3124,10 @@
         <v>43656</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="16">
         <v>1</v>
@@ -3104,7 +3136,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -3115,10 +3147,10 @@
         <v>43656</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" s="16">
         <v>1</v>
@@ -3127,7 +3159,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G8">
         <v>0.5</v>
@@ -3138,10 +3170,10 @@
         <v>43656</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -3150,7 +3182,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G9">
         <v>18</v>
@@ -3161,10 +3193,10 @@
         <v>43656</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -3173,7 +3205,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G10">
         <v>0.24660000000000001</v>
@@ -3382,20 +3414,20 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The size of any mobile inverts to the nearest millimeter. If more than one individual of a given taxon is present in a single quadrat, enter a single row for each individual." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="F1" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The qudrat meter point the sample was collected from: 1 - 50" sqref="E1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The size of any mobile inverts to the nearest millimeter. If more than one individual of a given taxon is present in a single quadrat, enter a single row for each individual." sqref="G1" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0400-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field" sqref="A1" xr:uid="{00000000-0002-0000-0400-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0400-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0400-000006000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -3422,143 +3454,143 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique identifier used to identify a single taxon. This column should include ALL uniquie TaxonID entries from the 'data' sheet" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indicate taxa's scientific name using standard scientific nomenclature." sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The unique identifier used to identify a single taxon. This column should include ALL uniquie TaxonID entries from the 'data' sheet" sqref="A1" xr:uid="{00000000-0002-0000-0500-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indicate taxa's scientific name using standard scientific nomenclature." sqref="B1" xr:uid="{00000000-0002-0000-0500-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -4579,14 +4611,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B21"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B31 B47"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1" xr:uid="{00000000-0002-0000-0600-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1" xr:uid="{00000000-0002-0000-0600-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{00000000-0002-0000-0600-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0600-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0600-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B21" xr:uid="{00000000-0002-0000-0600-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B31 B47" xr:uid="{00000000-0002-0000-0600-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>